<commit_message>
updating the mrb mc presentation
</commit_message>
<xml_diff>
--- a/doc/mrb_mc/mrb_data.xlsx
+++ b/doc/mrb_mc/mrb_data.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="14">
   <si>
     <t>Minimized Residual Batch Monte Carlo</t>
   </si>
@@ -96,6 +96,18 @@
   <si>
     <t>w_c = 1.0e-2</t>
   </si>
+  <si>
+    <t>Adjoint Monte Carlo</t>
+  </si>
+  <si>
+    <t>MCSA</t>
+  </si>
+  <si>
+    <t>Tolerance = 1.0e-8</t>
+  </si>
+  <si>
+    <t>MCSA Iterations</t>
+  </si>
 </sst>
 </file>
 
@@ -104,7 +116,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000E+00"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -148,29 +160,6 @@
       <u/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <i/>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
@@ -272,7 +261,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="71">
+  <cellStyleXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -344,18 +333,21 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -368,8 +360,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="71">
+  <cellStyles count="77">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -405,6 +401,9 @@
     <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -440,6 +439,9 @@
     <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -769,16 +771,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I53"/>
+  <dimension ref="A1:I56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
@@ -802,589 +804,800 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="16" thickBot="1"/>
+    <row r="7" spans="1:8" ht="16" thickBot="1">
+      <c r="A7" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
     <row r="8" spans="1:8" ht="16" thickTop="1">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="12"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="9"/>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="3" t="s">
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="14"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="11"/>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="13"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="4">
+      <c r="A10" s="10"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="5">
         <v>0</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="5">
         <v>0.01</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="5">
         <v>0.1</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F10" s="5">
         <v>1</v>
       </c>
-      <c r="G10" s="4">
+      <c r="G10" s="5">
         <v>10</v>
       </c>
-      <c r="H10" s="15">
+      <c r="H10" s="12">
         <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="13"/>
-      <c r="B11" s="4">
+      <c r="A11" s="10"/>
+      <c r="B11" s="5">
         <v>1</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="6">
         <v>8.4834209140500008</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="6">
         <v>1.89700658289</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="6">
         <v>0.70310262131199996</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="6">
         <v>0.39193007830499998</v>
       </c>
-      <c r="G11" s="5">
+      <c r="G11" s="6">
         <v>0.32879040222400002</v>
       </c>
-      <c r="H11" s="16">
+      <c r="H11" s="13">
         <v>0.272405117403</v>
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="13"/>
-      <c r="B12" s="4">
+      <c r="A12" s="10"/>
+      <c r="B12" s="5">
         <v>2</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="6">
         <v>8.4778222590999999</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="6">
         <v>1.89535721785</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12" s="6">
         <v>0.69071624310400004</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F12" s="6">
         <v>0.391920367474</v>
       </c>
-      <c r="G12" s="5">
+      <c r="G12" s="6">
         <v>0.32399489719300001</v>
       </c>
-      <c r="H12" s="16">
+      <c r="H12" s="13">
         <v>0.27199155195199998</v>
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="13"/>
-      <c r="B13" s="4">
+      <c r="A13" s="10"/>
+      <c r="B13" s="5">
         <v>5</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="6">
         <v>8.2309204655200006</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="6">
         <v>1.8788750244500001</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E13" s="6">
         <v>0.66843786172399999</v>
       </c>
-      <c r="F13" s="5">
+      <c r="F13" s="6">
         <v>0.37606368960499997</v>
       </c>
-      <c r="G13" s="5">
+      <c r="G13" s="6">
         <v>0.31277005303799998</v>
       </c>
-      <c r="H13" s="16">
+      <c r="H13" s="13">
         <v>0.266871867328</v>
       </c>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="17" t="s">
+      <c r="A14" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B14" s="4">
+      <c r="B14" s="5">
         <v>10</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C14" s="6">
         <v>7.6601997071700003</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="6">
         <v>1.7883489423900001</v>
       </c>
-      <c r="E14" s="5">
+      <c r="E14" s="6">
         <v>0.6490747107</v>
       </c>
-      <c r="F14" s="5">
+      <c r="F14" s="6">
         <v>0.36300335775699999</v>
       </c>
-      <c r="G14" s="5">
+      <c r="G14" s="6">
         <v>0.30760416592299999</v>
       </c>
-      <c r="H14" s="16">
+      <c r="H14" s="13">
         <v>0.25714155882200002</v>
       </c>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="13"/>
-      <c r="B15" s="4">
+      <c r="A15" s="10"/>
+      <c r="B15" s="5">
         <v>25</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C15" s="6">
         <v>6.5961155998400001</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D15" s="6">
         <v>1.62445881621</v>
       </c>
-      <c r="E15" s="5">
+      <c r="E15" s="6">
         <v>0.56745229353000004</v>
       </c>
-      <c r="F15" s="5">
+      <c r="F15" s="6">
         <v>0.33102431277400002</v>
       </c>
-      <c r="G15" s="5">
+      <c r="G15" s="6">
         <v>0.29361623903900003</v>
       </c>
-      <c r="H15" s="16">
+      <c r="H15" s="13">
         <v>0.24873886288700001</v>
       </c>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="13"/>
-      <c r="B16" s="4">
+      <c r="A16" s="10"/>
+      <c r="B16" s="5">
         <v>50</v>
       </c>
-      <c r="C16" s="5">
+      <c r="C16" s="6">
         <v>5.44658200756</v>
       </c>
-      <c r="D16" s="5">
+      <c r="D16" s="6">
         <v>1.1604653658599999</v>
       </c>
-      <c r="E16" s="5">
+      <c r="E16" s="6">
         <v>0.43782338279900002</v>
       </c>
-      <c r="F16" s="5">
+      <c r="F16" s="6">
         <v>0.27180696546900002</v>
       </c>
-      <c r="G16" s="5">
+      <c r="G16" s="6">
         <v>0.25801762101800002</v>
       </c>
-      <c r="H16" s="16">
+      <c r="H16" s="13">
         <v>0.195296871958</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="16" thickBot="1">
-      <c r="A17" s="18"/>
-      <c r="B17" s="19">
+      <c r="A17" s="15"/>
+      <c r="B17" s="16">
         <v>100</v>
       </c>
-      <c r="C17" s="20">
+      <c r="C17" s="17">
         <v>1.4046791183499999E-2</v>
       </c>
-      <c r="D17" s="20">
+      <c r="D17" s="17">
         <v>9.37555441379E-3</v>
       </c>
-      <c r="E17" s="20">
+      <c r="E17" s="17">
         <v>1.0032936138400001E-2</v>
       </c>
-      <c r="F17" s="20">
+      <c r="F17" s="17">
         <v>7.6760431282200002E-3</v>
       </c>
-      <c r="G17" s="20">
+      <c r="G17" s="17">
         <v>4.5450065053200001E-3</v>
       </c>
-      <c r="H17" s="21">
+      <c r="H17" s="18">
         <v>5.9410951619899999E-4</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="16" thickTop="1"/>
     <row r="19" spans="1:8" ht="16" thickBot="1"/>
     <row r="20" spans="1:8" ht="16" thickTop="1">
-      <c r="A20" s="10" t="s">
+      <c r="A20" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B20" s="11"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="12"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="9"/>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="13" t="s">
+      <c r="A21" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="3" t="s">
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="14"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="11"/>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="13"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="4">
+      <c r="A22" s="10"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="5">
         <v>0</v>
       </c>
-      <c r="D22" s="4">
+      <c r="D22" s="5">
         <v>0.01</v>
       </c>
-      <c r="E22" s="4">
+      <c r="E22" s="5">
         <v>0.1</v>
       </c>
-      <c r="F22" s="4">
+      <c r="F22" s="5">
         <v>1</v>
       </c>
-      <c r="G22" s="4">
+      <c r="G22" s="5">
         <v>10</v>
       </c>
-      <c r="H22" s="15">
+      <c r="H22" s="12">
         <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" s="13"/>
-      <c r="B23" s="4">
+      <c r="A23" s="10"/>
+      <c r="B23" s="5">
         <v>1</v>
       </c>
-      <c r="C23" s="5">
+      <c r="C23" s="6">
         <v>4.8790399137099998</v>
       </c>
-      <c r="D23" s="5">
+      <c r="D23" s="6">
         <v>1.10276658935</v>
       </c>
-      <c r="E23" s="5">
+      <c r="E23" s="6">
         <v>0.34098321898099998</v>
       </c>
-      <c r="F23" s="5">
+      <c r="F23" s="6">
         <v>0.172185386474</v>
       </c>
-      <c r="G23" s="5">
+      <c r="G23" s="6">
         <v>0.114242513236</v>
       </c>
-      <c r="H23" s="16">
+      <c r="H23" s="13">
         <v>0.12893199999999999</v>
       </c>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="13"/>
-      <c r="B24" s="4">
+      <c r="A24" s="10"/>
+      <c r="B24" s="5">
         <v>2</v>
       </c>
-      <c r="C24" s="5">
+      <c r="C24" s="6">
         <v>4.8509951624200003</v>
       </c>
-      <c r="D24" s="5">
+      <c r="D24" s="6">
         <v>1.1019896247700001</v>
       </c>
-      <c r="E24" s="5">
+      <c r="E24" s="6">
         <v>0.33967659247100002</v>
       </c>
-      <c r="F24" s="5">
+      <c r="F24" s="6">
         <v>0.152118783974</v>
       </c>
-      <c r="G24" s="5">
+      <c r="G24" s="6">
         <v>0.111186448435</v>
       </c>
-      <c r="H24" s="16">
+      <c r="H24" s="13">
         <v>0.128607360122</v>
       </c>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="13"/>
-      <c r="B25" s="4">
+      <c r="A25" s="10"/>
+      <c r="B25" s="5">
         <v>5</v>
       </c>
-      <c r="C25" s="5">
+      <c r="C25" s="6">
         <v>4.5340942484199998</v>
       </c>
-      <c r="D25" s="5">
+      <c r="D25" s="6">
         <v>0.843077143423</v>
       </c>
-      <c r="E25" s="5">
+      <c r="E25" s="6">
         <v>0.30910027364699999</v>
       </c>
-      <c r="F25" s="5">
+      <c r="F25" s="6">
         <v>0.156475268187</v>
       </c>
-      <c r="G25" s="5">
+      <c r="G25" s="6">
         <v>6.7866223592899996E-2</v>
       </c>
-      <c r="H25" s="16">
+      <c r="H25" s="13">
         <v>0.128607360122</v>
       </c>
     </row>
     <row r="26" spans="1:8">
-      <c r="A26" s="17" t="s">
+      <c r="A26" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B26" s="4">
+      <c r="B26" s="5">
         <v>10</v>
       </c>
-      <c r="C26" s="5">
+      <c r="C26" s="6">
         <v>4.3214486290099998</v>
       </c>
-      <c r="D26" s="5">
+      <c r="D26" s="6">
         <v>0.610686615401</v>
       </c>
-      <c r="E26" s="5">
+      <c r="E26" s="6">
         <v>0.23996382117000001</v>
       </c>
-      <c r="F26" s="5">
+      <c r="F26" s="6">
         <v>0.10337095052799999</v>
       </c>
-      <c r="G26" s="5">
+      <c r="G26" s="6">
         <v>5.7923851533400003E-2</v>
       </c>
-      <c r="H26" s="16">
+      <c r="H26" s="13">
         <v>0.100985864578</v>
       </c>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="13"/>
-      <c r="B27" s="4">
+      <c r="A27" s="10"/>
+      <c r="B27" s="5">
         <v>25</v>
       </c>
-      <c r="C27" s="5">
+      <c r="C27" s="6">
         <v>3.77427369291</v>
       </c>
-      <c r="D27" s="5">
+      <c r="D27" s="6">
         <v>0.471618025228</v>
       </c>
-      <c r="E27" s="5">
+      <c r="E27" s="6">
         <v>8.5319060350500006E-2</v>
       </c>
-      <c r="F27" s="5">
+      <c r="F27" s="6">
         <v>4.0885298248800002E-2</v>
       </c>
-      <c r="G27" s="5">
+      <c r="G27" s="6">
         <v>4.17952857323E-3</v>
       </c>
-      <c r="H27" s="16">
+      <c r="H27" s="13">
         <v>3.5761127512299999E-4</v>
       </c>
     </row>
     <row r="28" spans="1:8">
-      <c r="A28" s="13"/>
-      <c r="B28" s="4">
+      <c r="A28" s="10"/>
+      <c r="B28" s="5">
         <v>50</v>
       </c>
-      <c r="C28" s="5">
+      <c r="C28" s="6">
         <v>2.3464940087800001</v>
       </c>
-      <c r="D28" s="5">
+      <c r="D28" s="6">
         <v>0.31157563642699998</v>
       </c>
-      <c r="E28" s="5">
+      <c r="E28" s="6">
         <v>6.7652770718400002E-3</v>
       </c>
-      <c r="F28" s="5">
+      <c r="F28" s="6">
         <v>5.64346331089E-3</v>
       </c>
-      <c r="G28" s="5">
+      <c r="G28" s="6">
         <v>4.17952857323E-3</v>
       </c>
-      <c r="H28" s="16">
+      <c r="H28" s="13">
         <v>3.5761127512299999E-4</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="16" thickBot="1">
-      <c r="A29" s="18"/>
-      <c r="B29" s="19">
+      <c r="A29" s="15"/>
+      <c r="B29" s="16">
         <v>100</v>
       </c>
-      <c r="C29" s="20">
+      <c r="C29" s="17">
         <v>3.1621106731499998E-3</v>
       </c>
-      <c r="D29" s="20">
+      <c r="D29" s="17">
         <v>4.2124773524700003E-3</v>
       </c>
-      <c r="E29" s="20">
+      <c r="E29" s="17">
         <v>5.5546016384100004E-3</v>
       </c>
-      <c r="F29" s="20">
+      <c r="F29" s="17">
         <v>5.64346331089E-3</v>
       </c>
-      <c r="G29" s="20">
+      <c r="G29" s="17">
         <v>4.17952857323E-3</v>
       </c>
-      <c r="H29" s="21">
+      <c r="H29" s="18">
         <v>3.5761127512299999E-4</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="16" thickTop="1"/>
+    <row r="33" spans="1:9" ht="16" thickBot="1">
+      <c r="A33" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B33" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="16" thickTop="1">
+      <c r="A34" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B34" s="8"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="8"/>
+      <c r="E34" s="8"/>
+      <c r="F34" s="8"/>
+      <c r="G34" s="8"/>
+      <c r="H34" s="9"/>
+    </row>
+    <row r="35" spans="1:9">
+      <c r="A35" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="11"/>
+    </row>
+    <row r="36" spans="1:9">
+      <c r="A36" s="10"/>
+      <c r="B36" s="3"/>
+      <c r="C36" s="5">
+        <v>0</v>
+      </c>
+      <c r="D36" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="E36" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="F36" s="5">
+        <v>1</v>
+      </c>
+      <c r="G36" s="5">
+        <v>10</v>
+      </c>
+      <c r="H36" s="12">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
+      <c r="A37" s="10"/>
+      <c r="B37" s="5">
+        <v>1</v>
+      </c>
+      <c r="C37" s="19"/>
+      <c r="D37" s="19"/>
+      <c r="E37" s="19">
+        <v>16</v>
+      </c>
+      <c r="F37" s="19">
+        <v>10</v>
+      </c>
+      <c r="G37" s="19">
+        <v>6</v>
+      </c>
+      <c r="H37" s="20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
+      <c r="A38" s="10"/>
+      <c r="B38" s="5">
+        <v>2</v>
+      </c>
+      <c r="C38" s="19"/>
+      <c r="D38" s="19"/>
+      <c r="E38" s="19">
+        <v>16</v>
+      </c>
+      <c r="F38" s="19">
+        <v>10</v>
+      </c>
+      <c r="G38" s="19">
+        <v>6</v>
+      </c>
+      <c r="H38" s="20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9">
+      <c r="A39" s="10"/>
+      <c r="B39" s="5">
+        <v>5</v>
+      </c>
+      <c r="C39" s="19"/>
+      <c r="D39" s="19"/>
+      <c r="E39" s="19">
+        <v>16</v>
+      </c>
+      <c r="F39" s="19">
+        <v>10</v>
+      </c>
+      <c r="G39" s="19">
+        <v>6</v>
+      </c>
+      <c r="H39" s="20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
+      <c r="A40" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B40" s="5">
+        <v>10</v>
+      </c>
+      <c r="C40" s="19"/>
+      <c r="D40" s="19"/>
+      <c r="E40" s="19">
+        <v>16</v>
+      </c>
+      <c r="F40" s="19">
+        <v>10</v>
+      </c>
+      <c r="G40" s="19">
+        <v>6</v>
+      </c>
+      <c r="H40" s="20">
+        <v>4</v>
+      </c>
+    </row>
     <row r="41" spans="1:9">
-      <c r="A41" s="2"/>
-      <c r="B41" s="2"/>
-      <c r="C41" s="2"/>
-      <c r="D41" s="2"/>
-      <c r="E41" s="2"/>
-      <c r="F41" s="2"/>
-      <c r="G41" s="2"/>
-      <c r="H41" s="2"/>
-      <c r="I41" s="2"/>
+      <c r="A41" s="10"/>
+      <c r="B41" s="5">
+        <v>25</v>
+      </c>
+      <c r="C41" s="19"/>
+      <c r="D41" s="19"/>
+      <c r="E41" s="19">
+        <v>15</v>
+      </c>
+      <c r="F41" s="19">
+        <v>9</v>
+      </c>
+      <c r="G41" s="19">
+        <v>6</v>
+      </c>
+      <c r="H41" s="20">
+        <v>4</v>
+      </c>
+      <c r="I41" s="3"/>
     </row>
     <row r="42" spans="1:9">
-      <c r="A42" s="2"/>
-      <c r="B42" s="2"/>
-      <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
-      <c r="E42" s="2"/>
-      <c r="F42" s="2"/>
-      <c r="G42" s="2"/>
-      <c r="H42" s="2"/>
-      <c r="I42" s="2"/>
-    </row>
-    <row r="43" spans="1:9">
-      <c r="A43" s="2"/>
-      <c r="B43" s="2"/>
-      <c r="C43" s="2"/>
-      <c r="D43" s="2"/>
-      <c r="E43" s="2"/>
-      <c r="F43" s="2"/>
-      <c r="G43" s="2"/>
-      <c r="H43" s="2"/>
-      <c r="I43" s="2"/>
-    </row>
-    <row r="44" spans="1:9">
-      <c r="A44" s="6"/>
-      <c r="B44" s="6"/>
-      <c r="C44" s="6"/>
-      <c r="D44" s="6"/>
-      <c r="E44" s="6"/>
-      <c r="F44" s="6"/>
-      <c r="G44" s="6"/>
-      <c r="H44" s="6"/>
-      <c r="I44" s="2"/>
-    </row>
-    <row r="45" spans="1:9">
-      <c r="A45" s="6"/>
-      <c r="B45" s="6"/>
-      <c r="C45" s="6"/>
-      <c r="D45" s="6"/>
-      <c r="E45" s="7"/>
-      <c r="F45" s="6"/>
-      <c r="G45" s="6"/>
-      <c r="H45" s="6"/>
-      <c r="I45" s="2"/>
-    </row>
-    <row r="46" spans="1:9">
-      <c r="A46" s="6"/>
-      <c r="B46" s="6"/>
+      <c r="A42" s="10"/>
+      <c r="B42" s="5">
+        <v>50</v>
+      </c>
+      <c r="C42" s="19"/>
+      <c r="D42" s="19"/>
+      <c r="E42" s="19">
+        <v>14</v>
+      </c>
+      <c r="F42" s="19">
+        <v>9</v>
+      </c>
+      <c r="G42" s="19">
+        <v>5</v>
+      </c>
+      <c r="H42" s="20">
+        <v>4</v>
+      </c>
+      <c r="I42" s="3"/>
+    </row>
+    <row r="43" spans="1:9" ht="16" thickBot="1">
+      <c r="A43" s="15"/>
+      <c r="B43" s="16">
+        <v>100</v>
+      </c>
+      <c r="C43" s="21"/>
+      <c r="D43" s="21"/>
+      <c r="E43" s="21">
+        <v>4</v>
+      </c>
+      <c r="F43" s="21">
+        <v>4</v>
+      </c>
+      <c r="G43" s="21">
+        <v>3</v>
+      </c>
+      <c r="H43" s="22">
+        <v>2</v>
+      </c>
+      <c r="I43" s="3"/>
+    </row>
+    <row r="44" spans="1:9" ht="16" thickTop="1">
+      <c r="I44" s="3"/>
+    </row>
+    <row r="45" spans="1:9" ht="16" thickBot="1">
+      <c r="I45" s="3"/>
+    </row>
+    <row r="46" spans="1:9" ht="16" thickTop="1">
+      <c r="A46" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B46" s="8"/>
       <c r="C46" s="8"/>
       <c r="D46" s="8"/>
       <c r="E46" s="8"/>
       <c r="F46" s="8"/>
       <c r="G46" s="8"/>
-      <c r="H46" s="8"/>
-      <c r="I46" s="2"/>
+      <c r="H46" s="9"/>
+      <c r="I46" s="3"/>
     </row>
     <row r="47" spans="1:9">
-      <c r="A47" s="6"/>
-      <c r="B47" s="8"/>
-      <c r="C47" s="9"/>
-      <c r="D47" s="9"/>
-      <c r="E47" s="9"/>
-      <c r="F47" s="9"/>
-      <c r="G47" s="9"/>
-      <c r="H47" s="9"/>
-      <c r="I47" s="2"/>
+      <c r="A47" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B47" s="3"/>
+      <c r="C47" s="3"/>
+      <c r="D47" s="3"/>
+      <c r="E47" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F47" s="3"/>
+      <c r="G47" s="3"/>
+      <c r="H47" s="11"/>
+      <c r="I47" s="3"/>
     </row>
     <row r="48" spans="1:9">
-      <c r="A48" s="6"/>
-      <c r="B48" s="8"/>
-      <c r="C48" s="9"/>
-      <c r="D48" s="9"/>
-      <c r="E48" s="9"/>
-      <c r="F48" s="9"/>
-      <c r="G48" s="9"/>
-      <c r="H48" s="9"/>
-      <c r="I48" s="2"/>
+      <c r="A48" s="10"/>
+      <c r="B48" s="3"/>
+      <c r="C48" s="5">
+        <v>0</v>
+      </c>
+      <c r="D48" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="E48" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="F48" s="5">
+        <v>1</v>
+      </c>
+      <c r="G48" s="5">
+        <v>10</v>
+      </c>
+      <c r="H48" s="12">
+        <v>100</v>
+      </c>
+      <c r="I48" s="3"/>
     </row>
     <row r="49" spans="1:9">
-      <c r="A49" s="6"/>
-      <c r="B49" s="8"/>
-      <c r="C49" s="9"/>
-      <c r="D49" s="9"/>
-      <c r="E49" s="9"/>
-      <c r="F49" s="9"/>
-      <c r="G49" s="9"/>
-      <c r="H49" s="9"/>
-      <c r="I49" s="2"/>
+      <c r="A49" s="10"/>
+      <c r="B49" s="5">
+        <v>1</v>
+      </c>
+      <c r="C49" s="6"/>
+      <c r="D49" s="6"/>
+      <c r="E49" s="6"/>
+      <c r="F49" s="6"/>
+      <c r="G49" s="6"/>
+      <c r="H49" s="13"/>
+      <c r="I49" s="3"/>
     </row>
     <row r="50" spans="1:9">
-      <c r="A50" s="7"/>
-      <c r="B50" s="8"/>
-      <c r="C50" s="9"/>
-      <c r="D50" s="9"/>
-      <c r="E50" s="9"/>
-      <c r="F50" s="9"/>
-      <c r="G50" s="9"/>
-      <c r="H50" s="9"/>
-      <c r="I50" s="2"/>
+      <c r="A50" s="10"/>
+      <c r="B50" s="5">
+        <v>2</v>
+      </c>
+      <c r="C50" s="6"/>
+      <c r="D50" s="6"/>
+      <c r="E50" s="6"/>
+      <c r="F50" s="6"/>
+      <c r="G50" s="6"/>
+      <c r="H50" s="13"/>
+      <c r="I50" s="3"/>
     </row>
     <row r="51" spans="1:9">
-      <c r="A51" s="6"/>
-      <c r="B51" s="8"/>
-      <c r="C51" s="9"/>
-      <c r="D51" s="9"/>
-      <c r="E51" s="9"/>
-      <c r="F51" s="9"/>
-      <c r="G51" s="9"/>
-      <c r="H51" s="9"/>
-      <c r="I51" s="2"/>
+      <c r="A51" s="10"/>
+      <c r="B51" s="5">
+        <v>5</v>
+      </c>
+      <c r="C51" s="6"/>
+      <c r="D51" s="6"/>
+      <c r="E51" s="6"/>
+      <c r="F51" s="6"/>
+      <c r="G51" s="6"/>
+      <c r="H51" s="13"/>
+      <c r="I51" s="3"/>
     </row>
     <row r="52" spans="1:9">
-      <c r="A52" s="6"/>
-      <c r="B52" s="8"/>
-      <c r="C52" s="9"/>
-      <c r="D52" s="9"/>
-      <c r="E52" s="9"/>
-      <c r="F52" s="9"/>
-      <c r="G52" s="9"/>
-      <c r="H52" s="9"/>
-      <c r="I52" s="2"/>
+      <c r="A52" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B52" s="5">
+        <v>10</v>
+      </c>
+      <c r="C52" s="6"/>
+      <c r="D52" s="6"/>
+      <c r="E52" s="6"/>
+      <c r="F52" s="6"/>
+      <c r="G52" s="6"/>
+      <c r="H52" s="13"/>
+      <c r="I52" s="3"/>
     </row>
     <row r="53" spans="1:9">
-      <c r="A53" s="6"/>
-      <c r="B53" s="8"/>
-      <c r="C53" s="9"/>
-      <c r="D53" s="9"/>
-      <c r="E53" s="9"/>
-      <c r="F53" s="9"/>
-      <c r="G53" s="9"/>
-      <c r="H53" s="9"/>
-      <c r="I53" s="2"/>
-    </row>
+      <c r="A53" s="10"/>
+      <c r="B53" s="5">
+        <v>25</v>
+      </c>
+      <c r="C53" s="6"/>
+      <c r="D53" s="6"/>
+      <c r="E53" s="6"/>
+      <c r="F53" s="6"/>
+      <c r="G53" s="6"/>
+      <c r="H53" s="13"/>
+      <c r="I53" s="3"/>
+    </row>
+    <row r="54" spans="1:9">
+      <c r="A54" s="10"/>
+      <c r="B54" s="5">
+        <v>50</v>
+      </c>
+      <c r="C54" s="6"/>
+      <c r="D54" s="6"/>
+      <c r="E54" s="6"/>
+      <c r="F54" s="6"/>
+      <c r="G54" s="6"/>
+      <c r="H54" s="13"/>
+    </row>
+    <row r="55" spans="1:9" ht="16" thickBot="1">
+      <c r="A55" s="15"/>
+      <c r="B55" s="16">
+        <v>100</v>
+      </c>
+      <c r="C55" s="17"/>
+      <c r="D55" s="17"/>
+      <c r="E55" s="17"/>
+      <c r="F55" s="17"/>
+      <c r="G55" s="17"/>
+      <c r="H55" s="18"/>
+    </row>
+    <row r="56" spans="1:9" ht="16" thickTop="1"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>